<commit_message>
New data; indicator source treated as array, preventing big where same sources were shown multiple times on main vis
</commit_message>
<xml_diff>
--- a/datastatic/datasets/online/Employment_Youth_unemployment_rate_OECD_2013.xlsx
+++ b/datastatic/datasets/online/Employment_Youth_unemployment_rate_OECD_2013.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Employment_Youth_unemployment_rate_OECD_2013.csv" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="Employment_Youth_unemployment_r" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="95">
   <si>
     <t>original_title</t>
   </si>
@@ -94,27 +94,33 @@
     <t>target$explanation$de</t>
   </si>
   <si>
+    <t xml:space="preserve">Der Zielwert orientiert sich an den Ländern, die aktuell am besten abschneiden. </t>
+  </si>
+  <si>
+    <t>target$explanation$en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The target value is based on the currently best performing countries. </t>
+  </si>
+  <si>
+    <t>target$target_reference</t>
+  </si>
+  <si>
+    <t>target$tags</t>
+  </si>
+  <si>
+    <t>economic,social</t>
+  </si>
+  <si>
+    <t>target$target</t>
+  </si>
+  <si>
+    <t>target$ministerial_responsibility</t>
+  </si>
+  <si>
     <t>BMAS</t>
   </si>
   <si>
-    <t>target$explanation$en</t>
-  </si>
-  <si>
-    <t>target$target_reference</t>
-  </si>
-  <si>
-    <t>target$tags</t>
-  </si>
-  <si>
-    <t>economic,social</t>
-  </si>
-  <si>
-    <t>target$target</t>
-  </si>
-  <si>
-    <t>target$ministerial_responsibility</t>
-  </si>
-  <si>
     <t>target$other_relevant_SDGs</t>
   </si>
   <si>
@@ -124,24 +130,24 @@
     <t>scoring$timestamp</t>
   </si>
   <si>
-    <t>tbd</t>
-  </si>
-  <si>
     <t>scoring$type</t>
   </si>
   <si>
+    <t>national</t>
+  </si>
+  <si>
     <t>scoring$timestamp_data_host</t>
   </si>
   <si>
     <t>source</t>
   </si>
   <si>
-    <t>national</t>
-  </si>
-  <si>
     <t>source$type</t>
   </si>
   <si>
+    <t>inofficial</t>
+  </si>
+  <si>
     <t>source$note</t>
   </si>
   <si>
@@ -166,10 +172,10 @@
     <t>source$maintainer</t>
   </si>
   <si>
-    <t>inofficial</t>
-  </si>
-  <si>
     <t>source$license</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The OECD supports free use and consultation of its data by the public. Information source must be cited. Download is feasible. </t>
   </si>
   <si>
     <t>countries</t>
@@ -296,6 +302,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <sz val="10.0"/>
@@ -383,7 +392,7 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -551,23 +560,26 @@
       <c r="A18" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="B18" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>22</v>
@@ -575,88 +587,92 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="B25" s="8">
+        <v>42711.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="8">
-        <v>42306.0</v>
+        <v>39</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B27" s="2">
-        <v>2014.0</v>
+        <v>2015.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>41</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B28" s="2"/>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>51</v>
@@ -664,12 +680,15 @@
     </row>
     <row r="35">
       <c r="A35" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -696,7 +715,7 @@
     </row>
     <row r="38">
       <c r="A38" s="11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B38" s="12">
         <v>13.12868</v>
@@ -713,7 +732,7 @@
     </row>
     <row r="39">
       <c r="A39" s="11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B39" s="12">
         <v>10.575</v>
@@ -730,7 +749,7 @@
     </row>
     <row r="40">
       <c r="A40" s="11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B40" s="12">
         <v>22.1</v>
@@ -747,7 +766,7 @@
     </row>
     <row r="41">
       <c r="A41" s="11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="12">
@@ -762,7 +781,7 @@
     </row>
     <row r="42">
       <c r="A42" s="11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B42" s="12">
         <v>13.175</v>
@@ -779,7 +798,7 @@
     </row>
     <row r="43">
       <c r="A43" s="11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B43" s="12">
         <v>8.575</v>
@@ -796,7 +815,7 @@
     </row>
     <row r="44">
       <c r="A44" s="11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B44" s="12">
         <v>15.50438</v>
@@ -813,7 +832,7 @@
     </row>
     <row r="45">
       <c r="A45" s="11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B45" s="12">
         <v>12.55</v>
@@ -830,7 +849,7 @@
     </row>
     <row r="46">
       <c r="A46" s="11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B46" s="12">
         <v>7.25</v>
@@ -847,7 +866,7 @@
     </row>
     <row r="47">
       <c r="A47" s="11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B47" s="12">
         <v>10.85</v>
@@ -864,7 +883,7 @@
     </row>
     <row r="48">
       <c r="A48" s="11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B48" s="12">
         <v>22.35</v>
@@ -881,7 +900,7 @@
     </row>
     <row r="49">
       <c r="A49" s="11" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B49" s="12">
         <v>48.35</v>
@@ -898,7 +917,7 @@
     </row>
     <row r="50">
       <c r="A50" s="11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B50" s="12">
         <v>13.2</v>
@@ -915,7 +934,7 @@
     </row>
     <row r="51">
       <c r="A51" s="11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B51" s="12">
         <v>20.35</v>
@@ -932,7 +951,7 @@
     </row>
     <row r="52">
       <c r="A52" s="11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B52" s="12">
         <v>22.025</v>
@@ -949,7 +968,7 @@
     </row>
     <row r="53">
       <c r="A53" s="11" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B53" s="12">
         <v>24.675</v>
@@ -966,7 +985,7 @@
     </row>
     <row r="54">
       <c r="A54" s="11" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B54" s="12">
         <v>14.625</v>
@@ -983,7 +1002,7 @@
     </row>
     <row r="55">
       <c r="A55" s="11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B55" s="12">
         <v>49.8</v>
@@ -1000,7 +1019,7 @@
     </row>
     <row r="56">
       <c r="A56" s="11" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B56" s="12">
         <v>17.3</v>
@@ -1017,7 +1036,7 @@
     </row>
     <row r="57">
       <c r="A57" s="11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B57" s="12">
         <v>20.875</v>
@@ -1034,7 +1053,7 @@
     </row>
     <row r="58">
       <c r="A58" s="11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B58" s="12">
         <v>8.75</v>
@@ -1051,7 +1070,7 @@
     </row>
     <row r="59">
       <c r="A59" s="11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B59" s="12">
         <v>9.241667</v>
@@ -1068,7 +1087,7 @@
     </row>
     <row r="60">
       <c r="A60" s="11" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B60" s="12">
         <v>40.325</v>
@@ -1085,7 +1104,7 @@
     </row>
     <row r="61">
       <c r="A61" s="11" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B61" s="12">
         <v>5.575</v>
@@ -1102,7 +1121,7 @@
     </row>
     <row r="62">
       <c r="A62" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B62" s="12">
         <v>10.5208</v>
@@ -1119,7 +1138,7 @@
     </row>
     <row r="63">
       <c r="A63" s="11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B63" s="12">
         <v>17.325</v>
@@ -1136,7 +1155,7 @@
     </row>
     <row r="64">
       <c r="A64" s="11" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B64" s="12">
         <v>16.3</v>
@@ -1153,7 +1172,7 @@
     </row>
     <row r="65">
       <c r="A65" s="11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B65" s="12">
         <v>8.612964</v>
@@ -1170,7 +1189,7 @@
     </row>
     <row r="66">
       <c r="A66" s="11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B66" s="12">
         <v>11.25</v>
@@ -1187,7 +1206,7 @@
     </row>
     <row r="67">
       <c r="A67" s="11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B67" s="12">
         <v>9.875</v>
@@ -1204,7 +1223,7 @@
     </row>
     <row r="68">
       <c r="A68" s="11" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B68" s="12">
         <v>13.69827</v>
@@ -1221,7 +1240,7 @@
     </row>
     <row r="69">
       <c r="A69" s="11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B69" s="12">
         <v>13.87897</v>
@@ -1238,7 +1257,7 @@
     </row>
     <row r="70">
       <c r="A70" s="11" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B70" s="12">
         <v>20.75</v>
@@ -1255,7 +1274,7 @@
     </row>
     <row r="71">
       <c r="A71" s="11" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B71" s="12">
         <v>31.95</v>
@@ -1272,7 +1291,7 @@
     </row>
     <row r="72">
       <c r="A72" s="11" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B72" s="12">
         <v>26.45</v>
@@ -1289,7 +1308,7 @@
     </row>
     <row r="73">
       <c r="A73" s="11" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B73" s="12">
         <v>16.425</v>
@@ -1306,7 +1325,7 @@
     </row>
     <row r="74">
       <c r="A74" s="11" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B74" s="12">
         <v>20.325</v>
@@ -1323,7 +1342,7 @@
     </row>
     <row r="75">
       <c r="A75" s="11" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B75" s="12">
         <v>18.525</v>
@@ -1340,7 +1359,7 @@
     </row>
     <row r="76">
       <c r="A76" s="11" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B76" s="12">
         <v>11.6</v>
@@ -1357,7 +1376,7 @@
     </row>
     <row r="77">
       <c r="A77" s="11" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B77" s="12">
         <v>50.13005</v>

</xml_diff>